<commit_message>
added all types for submissions
</commit_message>
<xml_diff>
--- a/data/source/ieeevis-tw-rpi-edu/hcil-va-benchmark-tool-usage/version/2014-Jun-27/manual/submissions.rq.xlsx
+++ b/data/source/ieeevis-tw-rpi-edu/hcil-va-benchmark-tool-usage/version/2014-Jun-27/manual/submissions.rq.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="7360" windowWidth="28020" windowHeight="8300" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="6620" windowWidth="28080" windowHeight="10260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="submissions.rq.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="1144">
   <si>
     <t>submission</t>
   </si>
@@ -3491,15 +3491,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3729,54 +3721,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3790,9 +3797,11 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="23" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3803,6 +3812,18 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3813,9 +3834,252 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -3829,12 +4093,33 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4167,8 +4452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
-      <selection activeCell="G343" sqref="G343"/>
+    <sheetView tabSelected="1" topLeftCell="A341" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4455,7 +4740,9 @@
         <v>61</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E10" s="13" t="s">
         <v>722</v>
       </c>
@@ -4485,7 +4772,9 @@
         <v>459</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E11" s="5" t="s">
         <v>725</v>
       </c>
@@ -4519,7 +4808,9 @@
         <v>153</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E12" s="13" t="s">
         <v>731</v>
       </c>
@@ -4555,7 +4846,9 @@
         <v>521</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>735</v>
       </c>
@@ -4581,7 +4874,9 @@
         <v>571</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>736</v>
       </c>
@@ -4607,7 +4902,9 @@
         <v>47</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>691</v>
       </c>
@@ -4633,7 +4930,9 @@
         <v>75</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E16" s="5" t="s">
         <v>737</v>
       </c>
@@ -4659,7 +4958,9 @@
         <v>197</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E17" s="13" t="s">
         <v>738</v>
       </c>
@@ -4713,7 +5014,9 @@
         <v>437</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E19" s="13" t="s">
         <v>741</v>
       </c>
@@ -4739,7 +5042,7 @@
       <c r="A20" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="34" t="s">
         <v>325</v>
       </c>
       <c r="C20" s="5">
@@ -4763,11 +5066,13 @@
       <c r="A21" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="34" t="s">
         <v>177</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>744</v>
       </c>
@@ -4799,7 +5104,9 @@
         <v>365</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>707</v>
       </c>
@@ -4827,7 +5134,9 @@
         <v>441</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E23" s="5" t="s">
         <v>748</v>
       </c>
@@ -4853,7 +5162,9 @@
         <v>511</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E24" s="5" t="s">
         <v>749</v>
       </c>
@@ -4879,7 +5190,9 @@
         <v>115</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E25" s="5" t="s">
         <v>750</v>
       </c>
@@ -4907,7 +5220,9 @@
         <v>445</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E26" s="5" t="s">
         <v>752</v>
       </c>
@@ -4935,7 +5250,9 @@
         <v>495</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E27" s="5" t="s">
         <v>754</v>
       </c>
@@ -4963,7 +5280,9 @@
         <v>341</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>756</v>
       </c>
@@ -4989,7 +5308,9 @@
         <v>15</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E29" s="5" t="s">
         <v>703</v>
       </c>
@@ -5015,7 +5336,9 @@
         <v>185</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E30" s="5" t="s">
         <v>757</v>
       </c>
@@ -5041,7 +5364,9 @@
         <v>595</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E31" s="5" t="s">
         <v>758</v>
       </c>
@@ -5073,7 +5398,9 @@
         <v>315</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E32" s="5" t="s">
         <v>761</v>
       </c>
@@ -5127,7 +5454,9 @@
         <v>233</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E34" s="5" t="s">
         <v>694</v>
       </c>
@@ -5151,7 +5480,9 @@
         <v>335</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>715</v>
+      </c>
       <c r="E35" s="5" t="s">
         <v>763</v>
       </c>
@@ -5301,7 +5632,9 @@
         <v>545</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="E40" s="13" t="s">
         <v>775</v>
       </c>
@@ -5337,7 +5670,9 @@
         <v>39</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="E41" s="5" t="s">
         <v>805</v>
       </c>
@@ -6535,7 +6870,9 @@
         <v>375</v>
       </c>
       <c r="C79" s="5"/>
-      <c r="D79" s="4"/>
+      <c r="D79" s="4" t="s">
+        <v>697</v>
+      </c>
       <c r="E79" s="7" t="s">
         <v>707</v>
       </c>
@@ -8083,7 +8420,9 @@
         <v>663</v>
       </c>
       <c r="C130" s="5"/>
-      <c r="D130" s="4"/>
+      <c r="D130" s="4" t="s">
+        <v>693</v>
+      </c>
       <c r="E130" s="5" t="s">
         <v>694</v>
       </c>
@@ -8701,7 +9040,9 @@
         <v>231</v>
       </c>
       <c r="C151" s="5"/>
-      <c r="D151" s="4"/>
+      <c r="D151" s="4" t="s">
+        <v>693</v>
+      </c>
       <c r="E151" s="5" t="s">
         <v>694</v>
       </c>
@@ -9245,7 +9586,9 @@
         <v>29</v>
       </c>
       <c r="C169" s="5"/>
-      <c r="D169" s="4"/>
+      <c r="D169" s="4" t="s">
+        <v>701</v>
+      </c>
       <c r="E169" s="25" t="s">
         <v>904</v>
       </c>
@@ -11249,7 +11592,9 @@
         <v>381</v>
       </c>
       <c r="C235" s="5"/>
-      <c r="D235" s="4"/>
+      <c r="D235" s="4" t="s">
+        <v>695</v>
+      </c>
       <c r="E235" s="5" t="s">
         <v>694</v>
       </c>
@@ -14722,17 +15067,26 @@
     <sortCondition ref="B2:B343"/>
   </sortState>
   <conditionalFormatting sqref="E1:P43 E48:P48 G44:P46 F47:P47 E52:P52 G49:P49 K50:P50 G51:P51 E55:P55 G53:P54 E60:P62 M56:P56 E57 G57 K57:P57 F58:P58 G59:P59 E65:P66 H63:P63 F64:P64 E72:P72 F67:P67 G68:P68 F69:P69 E70 H70:P70 G71:P71 E76:P78 E73 G73:P73 H74:P74 F75:P75 E81:P81 G79:P80 E85:P87 E83 H82:P83 G84:P84 E90:P92 F88:P88 F89 H89:P89 E97:P97 F93:P93 F94:G94 I94:P94 F95:P95 G96:P96 E101:P101 F98:P100 E106:P106 I102:P102 F103:P103 E104 G104:P104 F105:P105 E108:P108 F107:P107 E111:P113 E109:F109 I109:P109 F110:P110 E115:P116 I114:P114 E124:P125 F117:P119 E120 G120:P121 F122:P123 E128:P128 I126:P126 H127:P127 E130:P130 G129:P129 E134:P134 F131 H131:P131 F132:P133 E136:P137 F135:P135 E146:P146 G138:P138 H139:P139 F140:P142 F143 H143:P143 F144:P145 E151:P151 F147 H147:P147 F148:P149 G150:P150 E154:P154 G152:P153 E156:P157 F155:P155 E160:P160 F158:P159 E162:P162 F161:P161 E165:P167 F163:P163 G164:P164 E170:P174 F168:P168 G169:P169 Q173 S173:U173 E176:P180 F175:P175 E182:P182 H181:P181 E184:P187 F183:P183 E190:P191 F188:P189 E193:P196 F192:P192 E198:P198 F197:P197 E200:P200 F199:P199 E202:P204 F201:P201 E206:P207 E205 G205:P205 E211:P222 F208:P210 E224:P235 F223:P223 Q234 E237:P239 F236:P236 E241:P243 F240:P240 E245:P248 F244:P244 E250:P270 F249:P249 E272:P292 E271:I271 K271:P271 E294:P295 F293:I293 K293:P293 E297:P310 F296:P296 E312:P323 F311:P311 E326:P341 E324:F324 H324:P324 F325:P325 Q327:V327 E343:P1048576 F342:P342">
-    <cfRule type="containsBlanks" dxfId="0" priority="4">
+    <cfRule type="containsBlanks" dxfId="27" priority="5">
       <formula>LEN(TRIM(E1))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsBlanks" dxfId="25" priority="1">
+      <formula>LEN(TRIM(D1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1"/>
+    <hyperlink ref="B21" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{956E0682-8641-2745-891B-1C13431F5FD5}">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{956E0682-8641-2745-891B-1C13431F5FD5}">
             <xm:f>NOT(ISERROR(SEARCH("-",E1)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>

</xml_diff>